<commit_message>
add comment and add datavalidation
</commit_message>
<xml_diff>
--- a/02-02/Book1.xlsx
+++ b/02-02/Book1.xlsx
@@ -12,6 +12,39 @@
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>老师: </author>
+  </authors>
+  <commentList>
+    <comment ref="F6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <b/>
+            <color indexed="81"/>
+            <sz val="9"/>
+          </rPr>
+          <t>老师: </t>
+        </r>
+        <r>
+          <rPr>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <color indexed="81"/>
+            <sz val="9"/>
+          </rPr>
+          <t>优秀</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1301,7 +1334,13 @@
   <conditionalFormatting sqref="J4:J9">
     <cfRule type="top10" dxfId="1" priority="1" rank="1"/>
   </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" sqref="D4:D9" type="list">
+      <formula1>"1班,2班,3班"</formula1>
+    </dataValidation>
+  </dataValidations>
   <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId4"/>
   <picture r:id="rId3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>